<commit_message>
from my snowleopard with my new Python
</commit_message>
<xml_diff>
--- a/universe/all_universe.xlsx
+++ b/universe/all_universe.xlsx
@@ -10,7 +10,8 @@
     <sheet name="CAC40" sheetId="1" r:id="rId1"/>
     <sheet name="SBF250" sheetId="2" r:id="rId2"/>
     <sheet name="MS190" sheetId="3" r:id="rId3"/>
-    <sheet name="sumup" sheetId="4" r:id="rId4"/>
+    <sheet name="idx" sheetId="5" r:id="rId4"/>
+    <sheet name="sumup" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5217" uniqueCount="2086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5292" uniqueCount="2118">
   <si>
     <t>AC.PA</t>
   </si>
@@ -6280,6 +6281,102 @@
   </si>
   <si>
     <t>MS190</t>
+  </si>
+  <si>
+    <t>^FCHI</t>
+  </si>
+  <si>
+    <t>^GSPC</t>
+  </si>
+  <si>
+    <t>^DJI</t>
+  </si>
+  <si>
+    <t>IDX</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>^IXIC</t>
+  </si>
+  <si>
+    <t>^FTSE</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>^GDAXI</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>^N225</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>CLM15.NYM</t>
+  </si>
+  <si>
+    <t>^BVSP</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>^GSPTSE</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>^MERV</t>
+  </si>
+  <si>
+    <t>^MXX</t>
+  </si>
+  <si>
+    <t>^ATX</t>
+  </si>
+  <si>
+    <t>^BFX</t>
+  </si>
+  <si>
+    <t>FTSEMIB.MI</t>
+  </si>
+  <si>
+    <t>^SSMI</t>
+  </si>
+  <si>
+    <t>^HIS</t>
+  </si>
+  <si>
+    <t>^SBF250</t>
+  </si>
+  <si>
+    <t>EURUSD=X</t>
+  </si>
+  <si>
+    <t>EURBRL=X</t>
+  </si>
+  <si>
+    <t>GBP=X</t>
+  </si>
+  <si>
+    <t>EURCHF=X</t>
+  </si>
+  <si>
+    <t>XAUUSD=X</t>
+  </si>
+  <si>
+    <t>HGJ15.CMX</t>
+  </si>
+  <si>
+    <t>^XAU</t>
   </si>
 </sst>
 </file>
@@ -6328,8 +6425,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6342,15 +6445,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -18137,9 +18246,380 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2093</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2095</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2097</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>2101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>2105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>2107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>2108</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>2109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>2113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>2115</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>2117</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E670"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>